<commit_message>
add proj13 booking process.
</commit_message>
<xml_diff>
--- a/proj13_demo/data/MY20-Demo-Matrix-V6.5.xlsx
+++ b/proj13_demo/data/MY20-Demo-Matrix-V6.5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\HD\MY20\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\bitbucket\hd-emea-test-script\proj13_demo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="241">
   <si>
     <t>Deployment</t>
   </si>
@@ -742,9 +742,6 @@
   </si>
   <si>
     <t>FLTRK</t>
-  </si>
-  <si>
-    <t>OTHER</t>
   </si>
 </sst>
 </file>
@@ -2050,10 +2047,10 @@
   <dimension ref="A1:AJ954"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG2" sqref="AG2"/>
+      <selection pane="bottomRight" activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -2109,6 +2106,7 @@
       <c r="AC1" s="136"/>
       <c r="AD1" s="136"/>
       <c r="AE1" s="136"/>
+      <c r="AF1" s="136"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
       <c r="L2" s="135" t="s">
@@ -2172,7 +2170,7 @@
         <v>240</v>
       </c>
       <c r="AF2" s="135" t="s">
-        <v>241</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:36" ht="15.75" customHeight="1" thickBot="1">
@@ -41001,10 +40999,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="Y1:AE1"/>
     <mergeCell ref="R1:X1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="Y1:AF1"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="D4:D19 D21:D31">

</xml_diff>

<commit_message>
fixed bikelist checking issue.
</commit_message>
<xml_diff>
--- a/proj13_demo/data/MY20-Demo-Matrix-V6.5.xlsx
+++ b/proj13_demo/data/MY20-Demo-Matrix-V6.5.xlsx
@@ -2047,10 +2047,10 @@
   <dimension ref="A1:AJ954"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AD4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB7" sqref="AB7"/>
+      <selection pane="bottomRight" activeCell="AG9" sqref="AG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -2106,7 +2106,7 @@
       <c r="AC1" s="136"/>
       <c r="AD1" s="136"/>
       <c r="AE1" s="136"/>
-      <c r="AF1" s="136"/>
+      <c r="AF1" s="135"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
       <c r="L2" s="135" t="s">
@@ -41002,7 +41002,7 @@
     <mergeCell ref="R1:X1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="Y1:AF1"/>
+    <mergeCell ref="Y1:AE1"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="D4:D19 D21:D31">

</xml_diff>